<commit_message>
made change on helpbook
</commit_message>
<xml_diff>
--- a/helpbook.xlsx
+++ b/helpbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\SoftUni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54444B79-CA9E-4737-A453-98490B3C779B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3427C75A-37CE-4663-9D9B-A9AB1C832457}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="3525" windowWidth="15375" windowHeight="7995" xr2:uid="{01BCE898-FA68-405B-A481-E374F5E5E0C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{01BCE898-FA68-405B-A481-E374F5E5E0C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>Синтаксис</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>дава ти думата на обратно</t>
+  </si>
+  <si>
+    <t>after -  git log - enter - q (to go back to writing)</t>
   </si>
 </sst>
 </file>
@@ -1187,7 +1190,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="69.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:2" ht="69.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A47" s="19" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="51" spans="1:2" ht="111.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A51" s="21" t="s">
         <v>84</v>

</xml_diff>